<commit_message>
classmarks.xlsx and table3 contain point names
</commit_message>
<xml_diff>
--- a/assign3/tables/classmarks.xlsx
+++ b/assign3/tables/classmarks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Points</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,6 +483,11 @@
       <c r="E2" t="n">
         <v>-5</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +507,11 @@
       <c r="E3" t="n">
         <v>5</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -516,6 +531,11 @@
       <c r="E4" t="n">
         <v>15</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,6 +555,11 @@
       <c r="E5" t="n">
         <v>25</v>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +579,11 @@
       <c r="E6" t="n">
         <v>35</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -573,6 +603,11 @@
       <c r="E7" t="n">
         <v>45</v>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -592,6 +627,11 @@
       <c r="E8" t="n">
         <v>55</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -611,6 +651,11 @@
       <c r="E9" t="n">
         <v>65</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -630,6 +675,11 @@
       <c r="E10" t="n">
         <v>75</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,6 +699,11 @@
       <c r="E11" t="n">
         <v>85</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -668,6 +723,11 @@
       <c r="E12" t="n">
         <v>95</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -686,6 +746,11 @@
       </c>
       <c r="E13" t="n">
         <v>105</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>